<commit_message>
New code for graphing several dataframes
</commit_message>
<xml_diff>
--- a/PriceEngineCounty.xlsx
+++ b/PriceEngineCounty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unamm\Documents\5th year\Thesis\GIT\EVsIreland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EACD108-B0C5-4187-BD52-C8D5F22743EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AFB07A-D127-4D74-B4BF-EA728D92C1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,6 +543,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>